<commit_message>
Moved IgnoreHeaderCount and IgnoreLastRowCount to the ExcelLib instead of global static variables
</commit_message>
<xml_diff>
--- a/Excel.UnitTest/Inputs/RowSpacingTest.xlsx
+++ b/Excel.UnitTest/Inputs/RowSpacingTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17874\source\repos\Lorefist5\Excel\Excel.UnitTest\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17874\Source\Repos\Lorefist5\Excel\Excel.UnitTest\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9281CC5-2F98-4BA0-A684-32EDC659A9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B86C10-516E-4A57-8945-C6713A3260E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="5280" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5510" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>